<commit_message>
Corrections 0903 (suite réunion 0803)
Ajout descriptions + corrections diverses 509533cd357862c6d63eaf825880ea47c75940b5
</commit_message>
<xml_diff>
--- a/ig/majKereval/StructureDefinition-ror-contact-function-contact.xlsx
+++ b/ig/majKereval/StructureDefinition-ror-contact-function-contact.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-08T07:58:39+00:00</t>
+    <t>2023-03-09T09:15:18+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -120,7 +120,7 @@
     <t>Context</t>
   </si>
   <si>
-    <t>extension:https://interop.esante.gouv.fr/ig/fhir/ror30/StructureDefinition/ror-contact-function-contact</t>
+    <t>extension:https://interop.esante.gouv.fr/ig/fhir/ror30/StructureDefinition/ror-healthcareservice-contact</t>
   </si>
   <si>
     <t>ID</t>

</xml_diff>